<commit_message>
Resueltos bugs de insercion por excel
</commit_message>
<xml_diff>
--- a/estudiantes.xlsx
+++ b/estudiantes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Nombre</t>
   </si>
@@ -38,24 +38,12 @@
     <t>Correo</t>
   </si>
   <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>jose@mail.com</t>
-  </si>
-  <si>
     <t>Caracas</t>
   </si>
   <si>
     <t>CNU</t>
   </si>
   <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>maria@mail.com</t>
-  </si>
-  <si>
     <t>Los Teques</t>
   </si>
   <si>
@@ -69,6 +57,51 @@
   </si>
   <si>
     <t>Forma_ingreso</t>
+  </si>
+  <si>
+    <t>Jose Rodriguez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria Gonzales </t>
+  </si>
+  <si>
+    <t>jose@gmail.com</t>
+  </si>
+  <si>
+    <t>maria@gmail.com</t>
+  </si>
+  <si>
+    <t>Ana Tovar</t>
+  </si>
+  <si>
+    <t>ana.tovar.j1@gmail.com</t>
+  </si>
+  <si>
+    <t>Guatire</t>
+  </si>
+  <si>
+    <t>Acta de Convenio</t>
+  </si>
+  <si>
+    <t>Carlos Zarraga</t>
+  </si>
+  <si>
+    <t>carldanzar@gmail.com</t>
+  </si>
+  <si>
+    <t>Guarenas</t>
+  </si>
+  <si>
+    <t>Samuel Robinson</t>
+  </si>
+  <si>
+    <t>Manuel Tirado</t>
+  </si>
+  <si>
+    <t>manuel@gmail.com</t>
+  </si>
+  <si>
+    <t>San Antonio de los Altos</t>
   </si>
 </sst>
 </file>
@@ -408,25 +441,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
     <col min="7" max="7" width="28.140625" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -438,60 +475,130 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>12345</v>
+        <v>26543421</v>
       </c>
       <c r="C2" s="1">
         <v>36170</v>
       </c>
       <c r="D2">
-        <v>12345</v>
+        <v>4140923467</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>22333</v>
+        <v>27123456</v>
       </c>
       <c r="C3" s="1">
         <v>36558</v>
       </c>
       <c r="D3">
-        <v>6789</v>
+        <v>4123233356</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G4" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>27513495</v>
+      </c>
+      <c r="C4" s="1">
+        <v>36290</v>
+      </c>
+      <c r="D4">
+        <v>4141879142</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>27716438</v>
+      </c>
+      <c r="C5" s="1">
+        <v>37075</v>
+      </c>
+      <c r="D5">
+        <v>4263050789</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>28311858</v>
+      </c>
+      <c r="C6" s="1">
+        <v>37235</v>
+      </c>
+      <c r="D6">
+        <v>4168359965</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="3"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="4"/>
@@ -500,8 +607,11 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>